<commit_message>
Adds proper trained model to the examples
</commit_message>
<xml_diff>
--- a/examples/input/model.xlsx
+++ b/examples/input/model.xlsx
@@ -6,16 +6,25 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Learning Factor" r:id="rId3" sheetId="1"/>
-    <sheet name="Tier 1" r:id="rId4" sheetId="2"/>
-    <sheet name="Tier 2" r:id="rId5" sheetId="3"/>
-    <sheet name="Tier 3" r:id="rId6" sheetId="4"/>
+    <sheet name="Коэффициент скорости обучения" r:id="rId3" sheetId="1"/>
+    <sheet name="Слой 1" r:id="rId4" sheetId="2"/>
+    <sheet name="Слой 2" r:id="rId5" sheetId="3"/>
+    <sheet name="Слой 3" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="9">
+  <si>
+    <t>Коэффициент скорости обучения</t>
+  </si>
+  <si>
+    <t>Количество входов</t>
+  </si>
+  <si>
+    <t>Размерность выходного слоя</t>
+  </si>
   <si>
     <t>pseudo()</t>
   </si>
@@ -84,15 +93,26 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
         <v>8.0</v>
       </c>
-      <c r="B2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -111,58 +131,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -170,119 +190,119 @@
         <v>0.3576712555614151</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>1.13164155419902</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
         <v>0.3412254737714669</v>
@@ -291,60 +311,60 @@
         <v>0.4703440958643332</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>0.3666089979818214</v>
@@ -353,119 +373,119 @@
         <v>0.4918144012066579</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
         <v>0.5</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H7" t="n">
         <v>0.4984169807029637</v>
@@ -477,22 +497,22 @@
         <v>0.4984169807029637</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q7" t="n">
         <v>0.4997051899161086</v>
@@ -503,34 +523,34 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K8" t="n">
         <v>0.497015288454921</v>
@@ -542,13 +562,13 @@
         <v>0.497015288454921</v>
       </c>
       <c r="N8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q8" t="n">
         <v>0.4993438471251996</v>
@@ -559,43 +579,43 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N9" t="n">
         <v>0.4984138732419991</v>
@@ -628,34 +648,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -663,572 +683,572 @@
         <v>0.357671255561415</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>1.13164155419902</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
         <v>0.3412254737714669</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>0.4703440958643332</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
         <v>0.3666089979818214</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
         <v>0.4918144012066579</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8" t="n">
         <v>0.5</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>0.4984169807029637</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
         <v>0.4984169807029637</v>
       </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H11" t="n">
         <v>0.4984169807029637</v>
       </c>
       <c r="I11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>0.497015288454921</v>
       </c>
       <c r="G12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G13" t="n">
         <v>0.497015288454921</v>
       </c>
       <c r="H13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H14" t="n">
         <v>0.497015288454921</v>
       </c>
       <c r="I14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>0.4984138732419991</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G16" t="n">
         <v>0.4984138732419991</v>
       </c>
       <c r="H16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H17" t="n">
         <v>0.4984138732419991</v>
       </c>
       <c r="I17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I18" t="n">
         <v>0.4465931443178643</v>
       </c>
       <c r="J18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J19" t="n">
         <v>0.4461025670407523</v>
@@ -1249,7 +1269,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">

</xml_diff>